<commit_message>
templates 0.6.3 & 0.7.0 processing fine; vocpub 4.6 valid
</commit_message>
<xml_diff>
--- a/templates/VocExcel-template-062.xlsx
+++ b/templates/VocExcel-template-062.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/rdflib/VocExcel/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AA81FA-F51F-7F43-AE2E-21CBF49C7370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EF040D-C494-E94C-8FCE-8129B00ACB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="1400" windowWidth="29260" windowHeight="20200" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9140" yWindow="1400" windowWidth="29260" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -1177,6 +1177,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1194,9 +1197,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1419,7 +1419,7 @@
   </sheetPr>
   <dimension ref="A1:K983"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -1530,7 +1530,7 @@
       <c r="H8" s="43"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
-      <c r="K8" s="64"/>
+      <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.15">
       <c r="A9" s="43"/>
@@ -2807,12 +2807,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.15">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="2" spans="1:4" s="39" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
@@ -5942,16 +5942,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.15">
       <c r="A2" s="35" t="s">
@@ -6343,16 +6343,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
@@ -6482,13 +6482,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
@@ -7855,7 +7855,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -7868,11 +7868,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="25" t="s">

</xml_diff>